<commit_message>
Waiting for Data Work
</commit_message>
<xml_diff>
--- a/Katys_Pendulum.xlsx
+++ b/Katys_Pendulum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbin/Documents/GitHub/Lab-Katers_Pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E50EF264-01EE-1944-8699-7B0943623412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7059DAA0-D424-594A-9E36-DB1A12722AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Katys_Pendulum_csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
   <si>
     <t>Run #1</t>
   </si>
@@ -102,6 +101,15 @@
   </si>
   <si>
     <t>SUMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance </t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Bottom</t>
   </si>
 </sst>
 </file>
@@ -671,63 +679,61 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Upright</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
-              <c:f>Katys_Pendulum_csv!$A$17:$A$26</c:f>
+              <c:f>Katys_Pendulum_csv!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -756,78 +762,109 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Katys_Pendulum_csv!$B$17:$B$26</c:f>
+              <c:f>Katys_Pendulum_csv!$B$17:$B$27</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>21.14811111111111</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.1148111111111101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.798100000000002</c:v>
+                  <c:v>2.0798100000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.5701</c:v>
+                  <c:v>2.05701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.4526</c:v>
+                  <c:v>2.0452599999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.429400000000001</c:v>
+                  <c:v>2.0429400000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.512599999999999</c:v>
+                  <c:v>2.0512600000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.659099999999999</c:v>
+                  <c:v>2.0659099999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.885000000000002</c:v>
+                  <c:v>2.0885000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.1614</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21.8674</c:v>
+                  <c:v>2.1161400000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1867399999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-071B-9F42-9A67-CAE3F1F53FB7}"/>
+              <c16:uniqueId val="{00000000-9D68-1940-A0D1-8733DA2A52AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Upside-Down</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
-              <c:f>Katys_Pendulum_csv!$A$17:$A$26</c:f>
+              <c:f>Katys_Pendulum_csv!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -856,54 +893,57 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Katys_Pendulum_csv!$C$17:$C$26</c:f>
+              <c:f>Katys_Pendulum_csv!$C$17:$C$27</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>21.11577777777778</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.1115777777777778</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.958600000000001</c:v>
+                  <c:v>2.0958600000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.8751</c:v>
+                  <c:v>2.08751</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.798100000000002</c:v>
+                  <c:v>2.0798100000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.787299999999998</c:v>
+                  <c:v>2.0787299999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.801300000000001</c:v>
+                  <c:v>2.08013</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.863</c:v>
+                  <c:v>2.0863</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.9758</c:v>
+                  <c:v>2.0975799999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.133700000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21.586600000000001</c:v>
+                  <c:v>2.1133700000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1586600000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-071B-9F42-9A67-CAE3F1F53FB7}"/>
+              <c16:uniqueId val="{00000001-9D68-1940-A0D1-8733DA2A52AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -915,14 +955,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="652053696"/>
-        <c:axId val="1777892672"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="652053696"/>
+        <c:axId val="382868208"/>
+        <c:axId val="382869888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="382868208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -940,6 +980,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [cm]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -977,15 +1077,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1777892672"/>
+        <c:crossAx val="382869888"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1777892672"/>
+        <c:axId val="382869888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,9 +1139,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652053696"/>
+        <c:crossAx val="382868208"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1055,7 +1152,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1689,23 +1786,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>264059</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>183773</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>256743</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>118435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>600609</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>12574</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>118140</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>103372</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E2CA48-24B6-1B48-AE02-9220A22F5178}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6408F941-83F6-0F4C-90A0-C86CB3DE385C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2023,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN26"/>
+  <dimension ref="A1:AN27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="101" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3720,114 +3817,210 @@
         <v>21.586555555555556</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>53</v>
       </c>
       <c r="B17">
-        <v>21.14811111111111</v>
+        <f>M17/10</f>
+        <v>2.1148111111111101</v>
       </c>
       <c r="C17">
+        <f>N17/10</f>
+        <v>2.1115777777777778</v>
+      </c>
+      <c r="M17">
+        <v>21.148111111111099</v>
+      </c>
+      <c r="N17">
         <v>21.11577777777778</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>63</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
+        <f t="shared" ref="B18:B27" si="19">M18/10</f>
+        <v>2.0798100000000002</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C27" si="20">N18/10</f>
+        <v>2.0958600000000001</v>
+      </c>
+      <c r="M18" s="2">
         <v>20.798100000000002</v>
       </c>
-      <c r="C18" s="2">
+      <c r="N18" s="2">
         <v>20.958600000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>73</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
+        <f t="shared" si="19"/>
+        <v>2.05701</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="20"/>
+        <v>2.08751</v>
+      </c>
+      <c r="M19" s="2">
         <v>20.5701</v>
       </c>
-      <c r="C19" s="2">
+      <c r="N19" s="2">
         <v>20.8751</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>83</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
+        <f t="shared" si="19"/>
+        <v>2.0452599999999999</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="20"/>
+        <v>2.0798100000000002</v>
+      </c>
+      <c r="M20" s="2">
         <v>20.4526</v>
       </c>
-      <c r="C20" s="2">
+      <c r="N20" s="2">
         <v>20.798100000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>93</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
+        <f t="shared" si="19"/>
+        <v>2.0429400000000002</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="20"/>
+        <v>2.0787299999999997</v>
+      </c>
+      <c r="M21" s="2">
         <v>20.429400000000001</v>
       </c>
-      <c r="C21" s="2">
+      <c r="N21" s="2">
         <v>20.787299999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>103</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
+        <f t="shared" si="19"/>
+        <v>2.0512600000000001</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="20"/>
+        <v>2.08013</v>
+      </c>
+      <c r="M22" s="2">
         <v>20.512599999999999</v>
       </c>
-      <c r="C22" s="2">
+      <c r="N22" s="2">
         <v>20.801300000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>113</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
+        <f t="shared" si="19"/>
+        <v>2.0659099999999997</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="20"/>
+        <v>2.0863</v>
+      </c>
+      <c r="M23" s="2">
         <v>20.659099999999999</v>
       </c>
-      <c r="C23" s="2">
+      <c r="N23" s="2">
         <v>20.863</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>123</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
+        <f t="shared" si="19"/>
+        <v>2.0885000000000002</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="20"/>
+        <v>2.0975799999999998</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="M24" s="2">
         <v>20.885000000000002</v>
       </c>
-      <c r="C24" s="2">
+      <c r="N24" s="2">
         <v>20.9758</v>
       </c>
-      <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>133</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
+        <f t="shared" si="19"/>
+        <v>2.1161400000000001</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="20"/>
+        <v>2.1133700000000002</v>
+      </c>
+      <c r="M25" s="2">
         <v>21.1614</v>
       </c>
-      <c r="C25" s="2">
+      <c r="N25" s="2">
         <v>21.133700000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>153</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27">
+        <f t="shared" si="19"/>
+        <v>2.1867399999999999</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="20"/>
+        <v>2.1586600000000002</v>
+      </c>
+      <c r="M27" s="2">
         <v>21.8674</v>
       </c>
-      <c r="C26" s="2">
+      <c r="N27" s="2">
         <v>21.586600000000001</v>
       </c>
     </row>

</xml_diff>